<commit_message>
made back a page
</commit_message>
<xml_diff>
--- a/PlayerSaveData.xlsx
+++ b/PlayerSaveData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daely\Documents\GitHub\TheSaviorofFarthingham\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CC12FD2-8F11-4AD5-B6E5-E541DAF3BC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4918A91F-1C5A-435B-A175-B7B8C36AE888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{385CCC2A-EA69-44CC-BAD8-2D4ECFEA9C71}"/>
   </bookViews>
@@ -440,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A455C85A-B204-49C9-8A67-29A9A882827E}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -524,6 +524,62 @@
         <v>16</v>
       </c>
     </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed excel doc and made the slider for all 7 skills
</commit_message>
<xml_diff>
--- a/PlayerSaveData.xlsx
+++ b/PlayerSaveData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daely\Documents\GitHub\TheSaviorofFarthingham\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4918A91F-1C5A-435B-A175-B7B8C36AE888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16A6827-7595-42AB-A92A-204590FAE483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{385CCC2A-EA69-44CC-BAD8-2D4ECFEA9C71}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>RTLastSaved</t>
+  </si>
+  <si>
+    <t>Intelligence</t>
   </si>
 </sst>
 </file>
@@ -440,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A455C85A-B204-49C9-8A67-29A9A882827E}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,16 +462,17 @@
     <col min="9" max="9" width="6.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.90625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,28 +507,31 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -577,6 +584,9 @@
         <v>0</v>
       </c>
       <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
         <v>0</v>
       </c>
     </row>

</xml_diff>